<commit_message>
I Added Libraries for the sensor and the LCD
</commit_message>
<xml_diff>
--- a/Material/SmartClock_Materialliste.xlsx
+++ b/Material/SmartClock_Materialliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/sai_ragavan_edu_gbssg_ch/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/sai_ragavan_edu_gbssg_ch/Documents/Dokumente/Schule/ims-t/IP/SmartClock/ims.project.smartclock/Material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="395" documentId="8_{462786D1-4C4F-43AD-9779-E11ABC312B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{528A2954-D53B-40BB-B8E7-07931350929D}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="8_{462786D1-4C4F-43AD-9779-E11ABC312B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0492E387-3810-47C3-B7D3-72EE3FC27B95}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4DF3711A-0043-4D27-B00E-AB9931E5E226}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4DF3711A-0043-4D27-B00E-AB9931E5E226}"/>
   </bookViews>
   <sheets>
     <sheet name="Materialliste" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -317,10 +317,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -722,10 +723,10 @@
   <dimension ref="C8:CQF57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -737,7 +738,7 @@
     <col min="11" max="11" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:11">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>0</v>
       </c>
@@ -766,7 +767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:11">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>1</v>
       </c>
@@ -796,7 +797,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="3:11">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>1</v>
       </c>
@@ -826,7 +827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="3:11">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>1</v>
       </c>
@@ -856,8 +857,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="3:11" ht="15" customHeight="1">
-      <c r="C12">
+    <row r="12" spans="3:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="8">
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -886,7 +887,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="3:11" ht="14.25" customHeight="1">
+    <row r="13" spans="3:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>1</v>
       </c>
@@ -916,7 +917,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="3:11">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>4</v>
       </c>
@@ -946,7 +947,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="3:11">
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>1</v>
       </c>
@@ -976,7 +977,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="3:11">
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>1</v>
       </c>
@@ -1006,7 +1007,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="3:11">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>1</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="3:11">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>1</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="3:11">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>1</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="3:11">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20">
         <f>SUM(C9:C19)</f>
         <v>14</v>
@@ -1103,22 +1104,22 @@
         <v>139.34999999999997</v>
       </c>
     </row>
-    <row r="27" spans="3:11">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="3:11">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="3:11">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="3:11">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="3:11">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
     </row>
-    <row r="47" spans="2468:2476">
+    <row r="47" spans="2468:2476" x14ac:dyDescent="0.25">
       <c r="CPX47" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1148,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="2468:2476">
+    <row r="48" spans="2468:2476" x14ac:dyDescent="0.25">
       <c r="CPX48">
         <v>1</v>
       </c>
@@ -1177,7 +1178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="2468:2476">
+    <row r="49" spans="2468:2476" x14ac:dyDescent="0.25">
       <c r="CPX49">
         <v>1</v>
       </c>
@@ -1207,7 +1208,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="2468:2476">
+    <row r="50" spans="2468:2476" x14ac:dyDescent="0.25">
       <c r="CPX50">
         <v>1</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="2468:2476" ht="42.75">
+    <row r="51" spans="2468:2476" ht="42.75" x14ac:dyDescent="0.25">
       <c r="CPX51">
         <v>1</v>
       </c>
@@ -1267,7 +1268,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="2468:2476" ht="42.75">
+    <row r="52" spans="2468:2476" ht="42.75" x14ac:dyDescent="0.25">
       <c r="CPX52">
         <v>1</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="2468:2476" ht="28.5">
+    <row r="53" spans="2468:2476" ht="28.5" x14ac:dyDescent="0.25">
       <c r="CPX53">
         <v>1</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="2468:2476">
+    <row r="54" spans="2468:2476" x14ac:dyDescent="0.25">
       <c r="CPX54">
         <v>4</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="2468:2476">
+    <row r="55" spans="2468:2476" x14ac:dyDescent="0.25">
       <c r="CPX55">
         <v>2</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="2468:2476">
+    <row r="56" spans="2468:2476" x14ac:dyDescent="0.25">
       <c r="CPX56">
         <v>1</v>
       </c>
@@ -1417,7 +1418,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="2468:2476">
+    <row r="57" spans="2468:2476" x14ac:dyDescent="0.25">
       <c r="CPX57">
         <f>SUM(CPX48:CPX56)</f>
         <v>13</v>
@@ -1452,15 +1453,16 @@
     <hyperlink ref="H19" r:id="rId20" xr:uid="{EA732135-343B-40BC-A625-192424EE4E9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
   <tableParts count="2">
-    <tablePart r:id="rId21"/>
     <tablePart r:id="rId22"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{5daf41bd-338c-4311-b1b0-e1299889c34b}" enabled="0" method="" siteId="{5daf41bd-338c-4311-b1b0-e1299889c34b}" removed="1"/>
+  <clbl:label id="{806a8f2b-28e4-44c4-ac01-7357a3a2b9e7}" enabled="1" method="Standard" siteId="{5daf41bd-338c-4311-b1b0-e1299889c34b}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>